<commit_message>
Created ALU in Logisim
</commit_message>
<xml_diff>
--- a/Documentation/ALU-Truth_Table.xlsx
+++ b/Documentation/ALU-Truth_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\TTL-Computer\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\Active\TTL-Computer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{744978F3-2725-4E0F-8E19-0E245A1AEDD8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACD53ED-BC92-456F-B108-1CE1EE0F5BC1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18372" windowHeight="6600" xr2:uid="{A9AA342D-15EB-4FC9-801C-1BAF9D09ED12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A9AA342D-15EB-4FC9-801C-1BAF9D09ED12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
   <si>
     <t>S0</t>
   </si>
@@ -209,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,15 +238,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,9 +248,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,7 +575,7 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,25 +701,25 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>0</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="A6" s="7">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -828,639 +816,639 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15" t="s">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small improvement in mcc
</commit_message>
<xml_diff>
--- a/Documentation/ALU-Truth_Table.xlsx
+++ b/Documentation/ALU-Truth_Table.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\Active\TTL-Computer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACD53ED-BC92-456F-B108-1CE1EE0F5BC1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B819AABD-83DD-4DA0-BC13-5FBE9004835C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A9AA342D-15EB-4FC9-801C-1BAF9D09ED12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{A9AA342D-15EB-4FC9-801C-1BAF9D09ED12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
   <si>
     <t>S0</t>
   </si>
@@ -76,6 +80,576 @@
   </si>
   <si>
     <t>A - 1</t>
+  </si>
+  <si>
+    <t>NOP(1)</t>
+  </si>
+  <si>
+    <t>0000000;</t>
+  </si>
+  <si>
+    <t>HALT(1)</t>
+  </si>
+  <si>
+    <t>0000001;</t>
+  </si>
+  <si>
+    <t>MOV A B(1)</t>
+  </si>
+  <si>
+    <t>0000010;</t>
+  </si>
+  <si>
+    <t>MOV A C(1)</t>
+  </si>
+  <si>
+    <t>0000011;</t>
+  </si>
+  <si>
+    <t>MOV A D(1)</t>
+  </si>
+  <si>
+    <t>0000100;</t>
+  </si>
+  <si>
+    <t>MOV B A(1)</t>
+  </si>
+  <si>
+    <t>0000101;</t>
+  </si>
+  <si>
+    <t>MOV B C(1)</t>
+  </si>
+  <si>
+    <t>0000110;</t>
+  </si>
+  <si>
+    <t>MOV B D(1)</t>
+  </si>
+  <si>
+    <t>0000111;</t>
+  </si>
+  <si>
+    <t>MOV C A(1)</t>
+  </si>
+  <si>
+    <t>0001000;</t>
+  </si>
+  <si>
+    <t>MOV C B(1)</t>
+  </si>
+  <si>
+    <t>0001001;</t>
+  </si>
+  <si>
+    <t>MOV C D(1)</t>
+  </si>
+  <si>
+    <t>0001010;</t>
+  </si>
+  <si>
+    <t>MOV D A(1)</t>
+  </si>
+  <si>
+    <t>0001011;</t>
+  </si>
+  <si>
+    <t>MOV D B(1)</t>
+  </si>
+  <si>
+    <t>0001100;</t>
+  </si>
+  <si>
+    <t>MOV D C(1)</t>
+  </si>
+  <si>
+    <t>0001101;</t>
+  </si>
+  <si>
+    <t>MVI A(2)</t>
+  </si>
+  <si>
+    <t>0001110;</t>
+  </si>
+  <si>
+    <t>MVI B(2)</t>
+  </si>
+  <si>
+    <t>0001111;</t>
+  </si>
+  <si>
+    <t>MVI C(2)</t>
+  </si>
+  <si>
+    <t>0010000;</t>
+  </si>
+  <si>
+    <t>MVI D(2)</t>
+  </si>
+  <si>
+    <t>0010001;</t>
+  </si>
+  <si>
+    <t>LD A(3)</t>
+  </si>
+  <si>
+    <t>0010010;</t>
+  </si>
+  <si>
+    <t>LD B(3)</t>
+  </si>
+  <si>
+    <t>0010011;</t>
+  </si>
+  <si>
+    <t>ST A(3)</t>
+  </si>
+  <si>
+    <t>0010110;</t>
+  </si>
+  <si>
+    <t>ST B(3)</t>
+  </si>
+  <si>
+    <t>0010111;</t>
+  </si>
+  <si>
+    <t>ADD A(1)</t>
+  </si>
+  <si>
+    <t>0011010;</t>
+  </si>
+  <si>
+    <t>ADD B(1)</t>
+  </si>
+  <si>
+    <t>1100001;</t>
+  </si>
+  <si>
+    <t>ADD C(1)</t>
+  </si>
+  <si>
+    <t>0011011;</t>
+  </si>
+  <si>
+    <t>ADD D(1)</t>
+  </si>
+  <si>
+    <t>0011100;</t>
+  </si>
+  <si>
+    <t>ADC A(1)</t>
+  </si>
+  <si>
+    <t>0011101;</t>
+  </si>
+  <si>
+    <t>ADC B(1)</t>
+  </si>
+  <si>
+    <t>1100010;</t>
+  </si>
+  <si>
+    <t>ADC C(1)</t>
+  </si>
+  <si>
+    <t>0011110;</t>
+  </si>
+  <si>
+    <t>ADC D(1)</t>
+  </si>
+  <si>
+    <t>0011111;</t>
+  </si>
+  <si>
+    <t>SUB A(1)</t>
+  </si>
+  <si>
+    <t>0100000;</t>
+  </si>
+  <si>
+    <t>SUB B(1)</t>
+  </si>
+  <si>
+    <t>1100011;</t>
+  </si>
+  <si>
+    <t>SUB C(1)</t>
+  </si>
+  <si>
+    <t>0100001;</t>
+  </si>
+  <si>
+    <t>SUB D(1)</t>
+  </si>
+  <si>
+    <t>0100010;</t>
+  </si>
+  <si>
+    <t>SBC A(1)</t>
+  </si>
+  <si>
+    <t>0100011;</t>
+  </si>
+  <si>
+    <t>SBC B(1)</t>
+  </si>
+  <si>
+    <t>1100100;</t>
+  </si>
+  <si>
+    <t>SBC C(1)</t>
+  </si>
+  <si>
+    <t>0100100;</t>
+  </si>
+  <si>
+    <t>SBC D(1)</t>
+  </si>
+  <si>
+    <t>0100101;</t>
+  </si>
+  <si>
+    <t>AND A(1)</t>
+  </si>
+  <si>
+    <t>0100110;</t>
+  </si>
+  <si>
+    <t>AND B(1)</t>
+  </si>
+  <si>
+    <t>1100101;</t>
+  </si>
+  <si>
+    <t>AND C(1)</t>
+  </si>
+  <si>
+    <t>0100111;</t>
+  </si>
+  <si>
+    <t>AND D(1)</t>
+  </si>
+  <si>
+    <t>0101000;</t>
+  </si>
+  <si>
+    <t>OR A(1)</t>
+  </si>
+  <si>
+    <t>0101001;</t>
+  </si>
+  <si>
+    <t>OR B(1)</t>
+  </si>
+  <si>
+    <t>1100110;</t>
+  </si>
+  <si>
+    <t>OR C(1)</t>
+  </si>
+  <si>
+    <t>0101010;</t>
+  </si>
+  <si>
+    <t>OR D(1)</t>
+  </si>
+  <si>
+    <t>0101011;</t>
+  </si>
+  <si>
+    <t>XOR A(1)</t>
+  </si>
+  <si>
+    <t>0101100;</t>
+  </si>
+  <si>
+    <t>XOR B(1)</t>
+  </si>
+  <si>
+    <t>0101101;</t>
+  </si>
+  <si>
+    <t>XOR C(1)</t>
+  </si>
+  <si>
+    <t>0101110;</t>
+  </si>
+  <si>
+    <t>XOR D(1)</t>
+  </si>
+  <si>
+    <t>0101111;</t>
+  </si>
+  <si>
+    <t>NOT A(1)</t>
+  </si>
+  <si>
+    <t>0110000;</t>
+  </si>
+  <si>
+    <t>NOT B(1)</t>
+  </si>
+  <si>
+    <t>0110001;</t>
+  </si>
+  <si>
+    <t>NOT C(1)</t>
+  </si>
+  <si>
+    <t>0110010;</t>
+  </si>
+  <si>
+    <t>NOT D(1)</t>
+  </si>
+  <si>
+    <t>0110011;</t>
+  </si>
+  <si>
+    <t>INC A(1)</t>
+  </si>
+  <si>
+    <t>0110100;</t>
+  </si>
+  <si>
+    <t>INC B(1)</t>
+  </si>
+  <si>
+    <t>0110101;</t>
+  </si>
+  <si>
+    <t>INC C(1)</t>
+  </si>
+  <si>
+    <t>0110110;</t>
+  </si>
+  <si>
+    <t>INC D(1)</t>
+  </si>
+  <si>
+    <t>0110111;</t>
+  </si>
+  <si>
+    <t>DEC A(1)</t>
+  </si>
+  <si>
+    <t>0111000;</t>
+  </si>
+  <si>
+    <t>DEC B(1)</t>
+  </si>
+  <si>
+    <t>0111001;</t>
+  </si>
+  <si>
+    <t>DEC C(1)</t>
+  </si>
+  <si>
+    <t>0111010;</t>
+  </si>
+  <si>
+    <t>DEC D(1)</t>
+  </si>
+  <si>
+    <t>0111011;</t>
+  </si>
+  <si>
+    <t>CMP(1)</t>
+  </si>
+  <si>
+    <t>0111100;</t>
+  </si>
+  <si>
+    <t>JMP(3)</t>
+  </si>
+  <si>
+    <t>0111111;</t>
+  </si>
+  <si>
+    <t>JZ(3)</t>
+  </si>
+  <si>
+    <t>1000000;</t>
+  </si>
+  <si>
+    <t>JN(3)</t>
+  </si>
+  <si>
+    <t>1000001;</t>
+  </si>
+  <si>
+    <t>JC(3)</t>
+  </si>
+  <si>
+    <t>1000010;</t>
+  </si>
+  <si>
+    <t>JNC(3)</t>
+  </si>
+  <si>
+    <t>1000011;</t>
+  </si>
+  <si>
+    <t>JEQ(3)</t>
+  </si>
+  <si>
+    <t>1000100;</t>
+  </si>
+  <si>
+    <t>JLT(3)</t>
+  </si>
+  <si>
+    <t>1000101;</t>
+  </si>
+  <si>
+    <t>JGT(3)</t>
+  </si>
+  <si>
+    <t>1000110;</t>
+  </si>
+  <si>
+    <t>CALL(3)</t>
+  </si>
+  <si>
+    <t>1000111;</t>
+  </si>
+  <si>
+    <t>RET(1)</t>
+  </si>
+  <si>
+    <t>1001000;</t>
+  </si>
+  <si>
+    <t>IN A(1)</t>
+  </si>
+  <si>
+    <t>1001001;</t>
+  </si>
+  <si>
+    <t>IN B(1)</t>
+  </si>
+  <si>
+    <t>1001010;</t>
+  </si>
+  <si>
+    <t>IN C(1)</t>
+  </si>
+  <si>
+    <t>1001011;</t>
+  </si>
+  <si>
+    <t>IN D(1)</t>
+  </si>
+  <si>
+    <t>1001100;</t>
+  </si>
+  <si>
+    <t>OUT 1 A(1)</t>
+  </si>
+  <si>
+    <t>1001101;</t>
+  </si>
+  <si>
+    <t>OUT 1 B(1)</t>
+  </si>
+  <si>
+    <t>1001110;</t>
+  </si>
+  <si>
+    <t>OUT 1 C(1)</t>
+  </si>
+  <si>
+    <t>1001111;</t>
+  </si>
+  <si>
+    <t>OUT 1 D(1)</t>
+  </si>
+  <si>
+    <t>1010000;</t>
+  </si>
+  <si>
+    <t>OUT 2 A(1)</t>
+  </si>
+  <si>
+    <t>1010001;</t>
+  </si>
+  <si>
+    <t>OUT 2 B(1)</t>
+  </si>
+  <si>
+    <t>1010010;</t>
+  </si>
+  <si>
+    <t>OUT 2 C(1)</t>
+  </si>
+  <si>
+    <t>1010011;</t>
+  </si>
+  <si>
+    <t>OUT 2 D(1)</t>
+  </si>
+  <si>
+    <t>1010100;</t>
+  </si>
+  <si>
+    <t>MOV A AX(1)</t>
+  </si>
+  <si>
+    <t>1010101;</t>
+  </si>
+  <si>
+    <t>MOV B AX(1)</t>
+  </si>
+  <si>
+    <t>1010110;</t>
+  </si>
+  <si>
+    <t>MOV C AX(1)</t>
+  </si>
+  <si>
+    <t>1010111;</t>
+  </si>
+  <si>
+    <t>MOV D AX(1)</t>
+  </si>
+  <si>
+    <t>1011000;</t>
+  </si>
+  <si>
+    <t>MOV A AY(1)</t>
+  </si>
+  <si>
+    <t>1011001;</t>
+  </si>
+  <si>
+    <t>MOV B AY(1)</t>
+  </si>
+  <si>
+    <t>1011010;</t>
+  </si>
+  <si>
+    <t>MOV C AY(1)</t>
+  </si>
+  <si>
+    <t>1011011;</t>
+  </si>
+  <si>
+    <t>MOV D AY(1)</t>
+  </si>
+  <si>
+    <t>1011100;</t>
+  </si>
+  <si>
+    <t>MVI AX(2)</t>
+  </si>
+  <si>
+    <t>1100111;</t>
+  </si>
+  <si>
+    <t>MVI AY(2)</t>
+  </si>
+  <si>
+    <t>1110000;</t>
   </si>
 </sst>
 </file>
@@ -574,18 +1148,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DC955E-4C83-4AB8-B34F-8247C50EF477}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.88671875" style="3"/>
-    <col min="7" max="7" width="10.44140625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="6" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="10.42578125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +1182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -631,7 +1205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>0</v>
       </c>
@@ -654,7 +1228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>0</v>
       </c>
@@ -677,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -700,7 +1274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>0</v>
       </c>
@@ -723,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -746,7 +1320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -769,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>0</v>
       </c>
@@ -792,7 +1366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>0</v>
       </c>
@@ -815,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>1</v>
       </c>
@@ -838,7 +1412,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -847,7 +1421,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -856,7 +1430,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -865,7 +1439,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -874,7 +1448,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -883,7 +1457,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -892,7 +1466,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -901,7 +1475,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -910,7 +1484,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -919,7 +1493,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -928,7 +1502,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -937,7 +1511,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -946,7 +1520,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -955,7 +1529,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -964,7 +1538,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -973,7 +1547,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -982,7 +1556,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -991,7 +1565,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1000,7 +1574,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1009,7 +1583,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1018,7 +1592,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1027,7 +1601,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1036,7 +1610,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1045,7 +1619,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1054,7 +1628,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1063,7 +1637,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1072,7 +1646,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1081,7 +1655,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1090,7 +1664,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1099,7 +1673,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1108,7 +1682,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1117,7 +1691,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1126,7 +1700,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1135,7 +1709,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1144,7 +1718,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1153,7 +1727,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1162,7 +1736,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1171,7 +1745,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1180,7 +1754,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1189,7 +1763,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1198,7 +1772,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1207,7 +1781,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1216,7 +1790,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1225,7 +1799,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1234,7 +1808,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1243,7 +1817,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1252,7 +1826,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1261,7 +1835,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1270,7 +1844,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1279,7 +1853,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1288,7 +1862,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1297,7 +1871,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1306,7 +1880,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1315,7 +1889,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1324,7 +1898,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1333,7 +1907,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1342,7 +1916,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1351,7 +1925,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1360,7 +1934,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1369,7 +1943,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1378,7 +1952,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1387,7 +1961,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1396,7 +1970,7 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1405,7 +1979,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1414,7 +1988,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1423,7 +1997,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1432,7 +2006,7 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1441,7 +2015,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1454,4 +2028,788 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A998F643-F595-4447-A982-C50F88A2B5C5}">
+  <dimension ref="A1:B95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>157</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>171</v>
+      </c>
+      <c r="B72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>175</v>
+      </c>
+      <c r="B74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>179</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>181</v>
+      </c>
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>187</v>
+      </c>
+      <c r="B80" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>189</v>
+      </c>
+      <c r="B81" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>193</v>
+      </c>
+      <c r="B83" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>195</v>
+      </c>
+      <c r="B84" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>197</v>
+      </c>
+      <c r="B85" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>199</v>
+      </c>
+      <c r="B86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>103</v>
+      </c>
+      <c r="B93" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>203</v>
+      </c>
+      <c r="B94" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>205</v>
+      </c>
+      <c r="B95" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{EED81A73-D707-4394-A986-797290744DA9}">
+    <sortState ref="A2:B95">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>